<commit_message>
added google maps plotter
</commit_message>
<xml_diff>
--- a/PF7111/TFB_20250307_378_DAS.xlsx
+++ b/PF7111/TFB_20250307_378_DAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mars/Documents/TPS/tps_py_tools/PF7111/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2450656E-D428-964C-80F2-532B0142DCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBAF3FB-4418-DD45-AA2A-739232AB5E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="920" windowWidth="14900" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13680" yWindow="1460" windowWidth="14900" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
+      <selection activeCell="A2" sqref="A2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -449,7 +449,7 @@
         <v>298.24687499999999</v>
       </c>
       <c r="C2">
-        <v>18.113648340775029</v>
+        <v>18.11364833999999</v>
       </c>
       <c r="D2" s="2">
         <v>3.6</v>
@@ -470,7 +470,7 @@
         <v>347.61250000000001</v>
       </c>
       <c r="C3">
-        <v>21.415392116134552</v>
+        <v>21.415392116</v>
       </c>
       <c r="D3" s="2">
         <v>2.7</v>
@@ -491,7 +491,7 @@
         <v>399.03750000000002</v>
       </c>
       <c r="C4">
-        <v>26.592446555444489</v>
+        <v>26.592446554999999</v>
       </c>
       <c r="D4" s="2">
         <v>2.8</v>
@@ -512,7 +512,7 @@
         <v>453.25625000000002</v>
       </c>
       <c r="C5">
-        <v>33.036333198593233</v>
+        <v>33.036333196000001</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
@@ -533,7 +533,7 @@
         <v>501.87812500000001</v>
       </c>
       <c r="C6">
-        <v>38.724609294964132</v>
+        <v>38.724609295500009</v>
       </c>
       <c r="D6" s="2">
         <v>3.3</v>
@@ -554,7 +554,7 @@
         <v>550.61562500000002</v>
       </c>
       <c r="C7">
-        <v>43.94655148952819</v>
+        <v>43.946551491999998</v>
       </c>
       <c r="D7" s="2">
         <v>3.4</v>
@@ -575,7 +575,7 @@
         <v>580.12187500000005</v>
       </c>
       <c r="C8">
-        <v>48.205900710309187</v>
+        <v>48.205900710000009</v>
       </c>
       <c r="D8" s="2">
         <v>2.7</v>
@@ -590,13 +590,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2303.25</v>
+        <v>2264.375</v>
       </c>
       <c r="B9">
-        <v>258.484375</v>
+        <v>250.91562500000001</v>
       </c>
       <c r="C9">
-        <v>14.94407406699713</v>
+        <v>14.198438577999999</v>
       </c>
       <c r="D9" s="2">
         <v>3</v>
@@ -617,7 +617,7 @@
         <v>199.09687500000001</v>
       </c>
       <c r="C10">
-        <v>10.993951604633491</v>
+        <v>10.9939516075</v>
       </c>
       <c r="D10" s="2">
         <v>3.7</v>
@@ -638,7 +638,7 @@
         <v>184.95937499999999</v>
       </c>
       <c r="C11">
-        <v>10.457792305764681</v>
+        <v>10.45779231</v>
       </c>
       <c r="D11" s="2">
         <v>2.5</v>
@@ -659,7 +659,7 @@
         <v>337.61250000000001</v>
       </c>
       <c r="C12">
-        <v>20.81688871274611</v>
+        <v>20.816888712499999</v>
       </c>
       <c r="D12" s="2">
         <v>4.0999999999999996</v>
@@ -680,7 +680,7 @@
         <v>392.17812500000002</v>
       </c>
       <c r="C13">
-        <v>26.38795789262009</v>
+        <v>26.387957891999999</v>
       </c>
       <c r="D13" s="2">
         <v>3.1</v>

</xml_diff>